<commit_message>
Updated Terms & Conditions
</commit_message>
<xml_diff>
--- a/UAT/docs/DSB_Proprietary Index submision.xlsx
+++ b/UAT/docs/DSB_Proprietary Index submision.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://etradingsoftware-my.sharepoint.com/personal/tony_birrell_etradingsoftware_com/Documents/DSB Product Commitee/CPs/DSB CP003/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony Birrell\Etrading Software\OneDrive - Etrading Software\DSB Product Commitee\CPs\DSB CP003\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Last Modified Date</t>
   </si>
@@ -164,12 +164,6 @@
     <t>PURPOSE</t>
   </si>
   <si>
-    <t>SERVICES</t>
-  </si>
-  <si>
-    <t>Once users are registered as Authorised requesters using this form, they will be able to request additions or amendments for the following enumerated Proprietary index lists:</t>
-  </si>
-  <si>
     <r>
       <t>·</t>
     </r>
@@ -245,9 +239,6 @@
     <t>ACCESS</t>
   </si>
   <si>
-    <t>Once registered, Authorised requesters can engage with the DSB via the DSB Proprietary Index submission Form that will be sent to the user along with confirmation of registration as an Authorised requester.</t>
-  </si>
-  <si>
     <t>USAGE</t>
   </si>
   <si>
@@ -281,30 +272,446 @@
     <t>Company LEI</t>
   </si>
   <si>
-    <t>The DSB Proprietary Index Change workflow will be accessible to Authorised requesters (first time users need to contact the product.management@ANNA-DSB.com for an Authorised Requester form).</t>
-  </si>
-  <si>
-    <t>The DSB Proprietary Index Change workflow is designed to provide a mechanism for industry representatives to engage with the DSB in adding new proprietary indices to the DSB enumerated list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The User (or its Affiliates) are prohibited from using this form to submit information that is subject to intellectual property constraints and acknowledge that the User is free to share the data with the DSB. The User (and its Affiliates) also acknowledge that any data provided to the DSB via this form is fully distributable to all users of the DSB as set out in the DSB Access and Usage Agreement and accompanying Policies. </t>
-  </si>
-  <si>
-    <t>Please note that these terms are subject to change and will be confirmed on 6 October 2017</t>
+    <t>The submission spreadsheet and associated workflow are designed to provide an efficient mechanism for industry representatives to engage with the DSB in adding new proprietary indices to the DSB enumerated list.</t>
+  </si>
+  <si>
+    <t>This submission process will only be accepted for the following asset classes:</t>
+  </si>
+  <si>
+    <t>The full suite of documentation for the process is &lt;available here&gt; and is comprised of:</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Authorized Requestor Registration Form</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DSB Proprietary Index Submission Form</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DSB Proprietary Index Change Workflow Description  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Only submissions made by Authorised Requesters will be accepted into the DSB’s Proprietary Index Change workflow</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Authorization must be sought no less than five working days in advance of submitting information - using the Authorized Requestor Registration Form, process described below</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Each organization wishing to participate in this process:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>must have at least one nominated administrator</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is responsible for maintaining its list of authorized users</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>will be allowed a maximum of six nominated users</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>must be a valid DSB User i.e. a signatory or named Affiliate as set out in the DSB Access and Usage Agreement</t>
+    </r>
+  </si>
+  <si>
+    <t>PROCESS:</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>On receipt of submissions, the DSB will update the publicly available list of enumerations via either GitHub or daily download file and will consist of the unique organisational prefix and index name only</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please note that enumerations cannot be deleted or amended</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Timing:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The DSB will endeavour to acknowledge and include on the “proprietary index master list” within 24 hours, although this is likely to be less</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>London working hours only with submissions ratified and included on the “proprietary index master list” between 9am and 6pm on a London business day</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If there is sufficient industry interest, the DSB could investigate significantly automating the submission process, thereby improving responsiveness</t>
+    </r>
+  </si>
+  <si>
+    <t>The User (or its Affiliates) are prohibited from using this form to submit information that is subject to intellectual property constraints and acknowledge that the User is free to share the data with the DSB. The User (and its Affiliates) also acknowledge that any data provided to the DSB via this form will remain fully distributable to all users of the DSB as set out in the DSB Access and Usage Agreement and accompanying Policies.</t>
+  </si>
+  <si>
+    <t>Furthermore, DSB data is available via file download to all users of the service and can be accessed, copied, reproduced, stored, distributed, disclosed, derived or otherwise communicated by any user of the DSB service, subject to the Third Party Data provision in the Acceptable Use Policy.</t>
+  </si>
+  <si>
+    <t>Please note that these terms may be subject to change</t>
+  </si>
+  <si>
+    <t>product.management@anna-dsb.com</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Authorised Requesters use the DSB Proprietary Index Submission Form to submit any additions to the proprietary index list must send the completed form to</t>
+    </r>
+  </si>
+  <si>
+    <t>Users submitting data to the DSB do so on behalf of the organisation for whom they are authorised requesters and by inference the authroised user's organisation complies with the usage terms above.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,9 +779,22 @@
     </font>
     <font>
       <b/>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -431,46 +851,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -801,10 +1229,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -842,8 +1270,8 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>28</v>
+      <c r="A5" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -852,8 +1280,8 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>29</v>
+      <c r="A6" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -871,49 +1299,49 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="E9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -928,103 +1356,223 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="147.42578125" customWidth="1"/>
+    <col min="1" max="1" width="147.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="35" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+    </row>
+    <row r="37" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="39" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>33</v>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A26" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>